<commit_message>
Product page files updated
</commit_message>
<xml_diff>
--- a/BenadrylAutomation/src/test/resources/TestData/ProdPageTestData.xlsx
+++ b/BenadrylAutomation/src/test/resources/TestData/ProdPageTestData.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="36">
   <si>
     <t>testcase</t>
   </si>
@@ -35,7 +35,7 @@
     <t>Verify the product title</t>
   </si>
   <si>
-    <t>BENADRYL® Allergy ULTRATABS® Tablets with Allergy Relief and Diphenhydramine HCI 25 mg</t>
+    <t>BENADRYLÂ® Allergy ULTRATABSÂ® Tablets with Allergy Relief and Diphenhydramine HCI 25 mg</t>
   </si>
   <si>
     <t>Verify the product rating</t>
@@ -47,13 +47,82 @@
     <t>Verify the "Write a Review" button</t>
   </si>
   <si>
-    <t xml:space="preserve">Write a review </t>
+    <t>Write a review</t>
   </si>
   <si>
     <t>Verify the "Buy Now" button</t>
   </si>
   <si>
     <t>BUY NOW</t>
+  </si>
+  <si>
+    <t>jumpToHeading</t>
+  </si>
+  <si>
+    <t>sectionHeading</t>
+  </si>
+  <si>
+    <t>Verify jumping to Overview</t>
+  </si>
+  <si>
+    <t>OVERVIEW</t>
+  </si>
+  <si>
+    <t>Product Overview</t>
+  </si>
+  <si>
+    <t>Verify jumping to Directions</t>
+  </si>
+  <si>
+    <t>DIRECTIONS</t>
+  </si>
+  <si>
+    <t>Directions</t>
+  </si>
+  <si>
+    <t>Verify jumping to Ingredients</t>
+  </si>
+  <si>
+    <t>INGREDIENTS</t>
+  </si>
+  <si>
+    <t>Ingredients</t>
+  </si>
+  <si>
+    <t>Verify jumping to Used For</t>
+  </si>
+  <si>
+    <t>USED FOR</t>
+  </si>
+  <si>
+    <t>Used For</t>
+  </si>
+  <si>
+    <t>Verify jumping to Warnings</t>
+  </si>
+  <si>
+    <t>WARNINGS</t>
+  </si>
+  <si>
+    <t>Warnings</t>
+  </si>
+  <si>
+    <t>Verify jumping to FAQs</t>
+  </si>
+  <si>
+    <t>FAQS</t>
+  </si>
+  <si>
+    <t>Frequently Asked Questions</t>
+  </si>
+  <si>
+    <t>Verify jumping to Review</t>
+  </si>
+  <si>
+    <t>REVIEWS</t>
+  </si>
+  <si>
+    <t>Reviews</t>
   </si>
 </sst>
 </file>
@@ -667,16 +736,10 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1000,22 +1063,22 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:C1"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="6" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="6" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="28.8857142857143" style="2" customWidth="1"/>
-    <col min="2" max="2" width="11.6666666666667" style="2" customWidth="1"/>
-    <col min="3" max="3" width="30.2857142857143" style="2" customWidth="1"/>
-    <col min="4" max="4" width="17.2190476190476" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="9" style="2"/>
+    <col min="1" max="1" width="28.8857142857143" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6666666666667" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.2857142857143" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.2190476190476" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1025,31 +1088,28 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1"/>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="3" t="s">
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" ht="45" spans="1:3">
-      <c r="A3" s="3" t="s">
+    </row>
+    <row r="3" ht="60" spans="1:3">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1057,7 +1117,7 @@
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1065,24 +1125,24 @@
       </c>
     </row>
     <row r="6" ht="30" spans="1:3">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1095,20 +1155,20 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="7" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="21.5714285714286" customWidth="1"/>
     <col min="2" max="2" width="12.1428571428571" customWidth="1"/>
     <col min="3" max="3" width="18.8571428571429" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1116,7 +1176,108 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" ht="30" spans="1:4">
+      <c r="A2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" ht="30" spans="1:4">
+      <c r="A3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" ht="30" spans="1:4">
+      <c r="A4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" ht="30" spans="1:4">
+      <c r="A5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" ht="30" spans="1:4">
+      <c r="A6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" ht="30" spans="1:4">
+      <c r="A8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated based on the comments in the PR
</commit_message>
<xml_diff>
--- a/BenadrylAutomation/src/test/resources/TestData/ProdPageTestData.xlsx
+++ b/BenadrylAutomation/src/test/resources/TestData/ProdPageTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12330" activeTab="1"/>
+    <workbookView windowWidth="28800" windowHeight="12330" firstSheet="4" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="prodImg" sheetId="3" r:id="rId1"/>
@@ -19,13 +19,14 @@
     <sheet name="jumpToWarnings" sheetId="10" r:id="rId10"/>
     <sheet name="jumpToFAQs" sheetId="11" r:id="rId11"/>
     <sheet name="jumpToReviews" sheetId="12" r:id="rId12"/>
+    <sheet name="jumpTo" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="38">
   <si>
     <t>testcase</t>
   </si>
@@ -156,7 +157,13 @@
     <t>Frequently Asked Questions</t>
   </si>
   <si>
+    <t>Verify jumping to Reviews</t>
+  </si>
+  <si>
     <t>REVIEWS</t>
+  </si>
+  <si>
+    <t>Reviews</t>
   </si>
 </sst>
 </file>
@@ -1149,7 +1156,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="$A3:$XFD1048576"/>
+      <selection activeCell="C2" sqref="C2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="3"/>
@@ -1199,7 +1206,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C2" sqref="C2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="3"/>
@@ -1249,7 +1256,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="2"/>
@@ -1265,15 +1272,149 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" ht="45" spans="1:3">
+    <row r="2" ht="60" spans="1:3">
       <c r="A2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="7" outlineLevelCol="3"/>
+  <cols>
+    <col min="1" max="1" width="19.2857142857143" customWidth="1"/>
+    <col min="2" max="2" width="21.7142857142857" customWidth="1"/>
+    <col min="3" max="4" width="18.7142857142857" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" ht="30" spans="1:4">
+      <c r="A2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" ht="30" spans="1:4">
+      <c r="A3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" ht="30" spans="1:4">
+      <c r="A4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" ht="30" spans="1:4">
+      <c r="A5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" ht="30" spans="1:4">
+      <c r="A6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" ht="30" spans="1:4">
+      <c r="A7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" ht="30" spans="1:4">
+      <c r="A8" s="2" t="s">
         <v>35</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1287,7 +1428,7 @@
   <sheetPr/>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1453,7 +1594,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C2" sqref="C2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="3"/>
@@ -1503,7 +1644,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C2" sqref="C2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="3"/>
@@ -1553,7 +1694,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C2" sqref="C2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="3"/>
@@ -1603,7 +1744,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C2" sqref="C2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="3"/>

</xml_diff>

<commit_message>
PDP updated according to PR comments
</commit_message>
<xml_diff>
--- a/BenadrylAutomation/src/test/resources/TestData/ProdPageTestData.xlsx
+++ b/BenadrylAutomation/src/test/resources/TestData/ProdPageTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12330" firstSheet="4" activeTab="12"/>
+    <workbookView windowWidth="28800" windowHeight="12330" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="prodImg" sheetId="3" r:id="rId1"/>
@@ -12,21 +12,14 @@
     <sheet name="prodRating" sheetId="5" r:id="rId3"/>
     <sheet name="prodOverview" sheetId="6" r:id="rId4"/>
     <sheet name="prodPageBtns" sheetId="1" r:id="rId5"/>
-    <sheet name="jumpToOverview" sheetId="2" r:id="rId6"/>
-    <sheet name="jumpToDirections" sheetId="7" r:id="rId7"/>
-    <sheet name="jumpToIngredients" sheetId="8" r:id="rId8"/>
-    <sheet name="jumpToUsed" sheetId="9" r:id="rId9"/>
-    <sheet name="jumpToWarnings" sheetId="10" r:id="rId10"/>
-    <sheet name="jumpToFAQs" sheetId="11" r:id="rId11"/>
-    <sheet name="jumpToReviews" sheetId="12" r:id="rId12"/>
-    <sheet name="jumpTo" sheetId="13" r:id="rId13"/>
+    <sheet name="jumpTo" sheetId="13" r:id="rId6"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="38">
   <si>
     <t>testcase</t>
   </si>
@@ -1150,279 +1143,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="3"/>
-  <cols>
-    <col min="1" max="1" width="21.5714285714286" customWidth="1"/>
-    <col min="2" max="2" width="12.1428571428571" customWidth="1"/>
-    <col min="3" max="3" width="18.8571428571429" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" ht="30" spans="1:4">
-      <c r="A2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="3"/>
-  <cols>
-    <col min="1" max="1" width="21.5714285714286" customWidth="1"/>
-    <col min="2" max="2" width="12.1428571428571" customWidth="1"/>
-    <col min="3" max="3" width="18.8571428571429" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="2"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" ht="60" spans="1:3">
-      <c r="A2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:D8"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="7" outlineLevelCol="3"/>
-  <cols>
-    <col min="1" max="1" width="19.2857142857143" customWidth="1"/>
-    <col min="2" max="2" width="21.7142857142857" customWidth="1"/>
-    <col min="3" max="4" width="18.7142857142857" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" ht="30" spans="1:4">
-      <c r="A2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" ht="30" spans="1:4">
-      <c r="A3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" ht="30" spans="1:4">
-      <c r="A4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" ht="30" spans="1:4">
-      <c r="A5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" ht="30" spans="1:4">
-      <c r="A6" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" ht="30" spans="1:4">
-      <c r="A7" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" ht="30" spans="1:4">
-      <c r="A8" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
@@ -1591,17 +1311,17 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="7" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="21.5714285714286" customWidth="1"/>
-    <col min="2" max="2" width="12.1428571428571" customWidth="1"/>
-    <col min="3" max="3" width="18.8571428571429" customWidth="1"/>
+    <col min="1" max="1" width="19.2857142857143" customWidth="1"/>
+    <col min="2" max="2" width="21.7142857142857" customWidth="1"/>
+    <col min="3" max="4" width="18.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1632,154 +1352,88 @@
         <v>19</v>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="3"/>
-  <cols>
-    <col min="1" max="1" width="21.5714285714286" customWidth="1"/>
-    <col min="2" max="2" width="12.1428571428571" customWidth="1"/>
-    <col min="3" max="3" width="18.8571428571429" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" ht="30" spans="1:4">
-      <c r="A2" s="2" t="s">
+    <row r="3" ht="30" spans="1:4">
+      <c r="A3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>21</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D3" t="s">
         <v>22</v>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="3"/>
-  <cols>
-    <col min="1" max="1" width="21.5714285714286" customWidth="1"/>
-    <col min="2" max="2" width="12.1428571428571" customWidth="1"/>
-    <col min="3" max="3" width="18.8571428571429" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" ht="30" spans="1:4">
-      <c r="A2" s="2" t="s">
+    <row r="4" ht="30" spans="1:4">
+      <c r="A4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C4" t="s">
         <v>24</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D4" t="s">
         <v>25</v>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="3"/>
-  <cols>
-    <col min="1" max="1" width="21.5714285714286" customWidth="1"/>
-    <col min="2" max="2" width="12.1428571428571" customWidth="1"/>
-    <col min="3" max="3" width="18.8571428571429" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" ht="30" spans="1:4">
-      <c r="A2" s="2" t="s">
+    <row r="5" ht="30" spans="1:4">
+      <c r="A5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C5" t="s">
         <v>27</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D5" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="6" ht="30" spans="1:4">
+      <c r="A6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" ht="30" spans="1:4">
+      <c r="A7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" ht="30" spans="1:4">
+      <c r="A8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>